<commit_message>
project - datacleaning, 27:49
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Data-Analysis-Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9237F2D-0D16-4C46-8857-B76C23607BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFA126E-86E8-4F01-8E1E-A99E3840528C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Day #</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>NIL</t>
+  </si>
+  <si>
+    <t>Project 1</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +547,12 @@
       <c r="B9" s="1">
         <v>45870</v>
       </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">

</xml_diff>

<commit_message>
project - datacleaning, completed
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Data-Analysis-Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFA126E-86E8-4F01-8E1E-A99E3840528C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19627AB3-C41C-48EB-B976-971BB875CC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Day #</t>
   </si>
@@ -411,7 +411,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +561,12 @@
       <c r="B10" s="1">
         <v>45871</v>
       </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">

</xml_diff>

<commit_message>
project - EDA, completed
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Data-Analysis-Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19627AB3-C41C-48EB-B976-971BB875CC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B845FBD8-8131-4D67-8819-331522B1FE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Day #</t>
   </si>
@@ -66,7 +66,13 @@
     <t>NIL</t>
   </si>
   <si>
-    <t>Project 1</t>
+    <t>Data Cleaning Project</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>EDA Project</t>
   </si>
 </sst>
 </file>
@@ -410,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,11 +567,11 @@
       <c r="B10" s="1">
         <v>45871</v>
       </c>
-      <c r="C10">
-        <v>19</v>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -574,6 +580,12 @@
       </c>
       <c r="B11" s="1">
         <v>45872</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bins and calculated fields
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Data-Analysis-Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBBD882-737B-4D65-803C-B947D2BA4779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D429C81E-A7E9-4F05-930E-281B0C4AAC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Day #</t>
   </si>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +753,12 @@
       <c r="B22" s="1">
         <v>45883</v>
       </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -761,6 +767,12 @@
       <c r="B23" s="1">
         <v>45884</v>
       </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -769,6 +781,12 @@
       <c r="B24" s="1">
         <v>45885</v>
       </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -776,6 +794,12 @@
       </c>
       <c r="B25" s="1">
         <v>45886</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lec 60: grouping and aggregates
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -116,7 +116,7 @@
     <t>Pandas</t>
   </si>
   <si>
-    <t>indexing in pandas</t>
+    <t>group by, agg</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
         <v>45901</v>
       </c>
       <c r="C40">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>

</xml_diff>